<commit_message>
sucesso em salvar os dados da primeira empresa
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,44 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Nota</t>
+          <t>Reclamações Respondidas</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Reclamações Respondidas</t>
+          <t>Voltariam a Fazer Negócio</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Voltariam a Fazer Negócio</t>
+          <t>Índice de Solução</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Índice de Solução</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Nota do Consumidor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Respondeu 99.9% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 62.8% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 67.7% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como BOM. A nota média nos últimos 6 meses é 7.0/10.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Codigo final com todas as funcionalidades.
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,44 +436,224 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Empresa</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Reclamações Respondidas</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Voltariam a Fazer Negócio</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Índice de Solução</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Nota do Consumidor</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Classificação</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Shein</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>Respondeu 99.9% das reclamações recebidas.</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Dos que avaliaram, 62.8% voltariam a fazer negócio.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>A empresa resolveu 67.7% das reclamações recebidas.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>O consumidor avaliou o atendimento dessa empresa como BOM. A nota média nos últimos 6 meses é 7.0/10.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1º Melhor</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Centauro</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Respondeu 100% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 61% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 82% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como BOM. A nota média nos últimos 6 meses é 7.4/10.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2º Melhor</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lojas Renner</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Respondeu 99.9% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 80% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 89.6% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como ÓTIMO. A nota média nos últimos 6 meses é 8.5/10.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>3º Melhor</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Yeesco</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Respondeu 59.9% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 9.1% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 20.5% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como Não Recomendada. A nota média nos últimos 6 meses é 2.3/10.</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>1º Pior</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>bycih store</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Respondeu 99.8% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 13.1% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 37.3% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como Não Recomendada. A nota média nos últimos 6 meses é 3.9/10.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2º Pior</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Miazzi</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Respondeu 99.7% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dos que avaliaram, 5.4% voltariam a fazer negócio.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>A empresa resolveu 12% das reclamações recebidas.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>O consumidor avaliou o atendimento dessa empresa como Não Recomendada. A nota média nos últimos 6 meses é 2.7/10.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>3º Pior</t>
         </is>
       </c>
     </row>

</xml_diff>